<commit_message>
Update version to 2.0.0
</commit_message>
<xml_diff>
--- a/LocalizationTest.xlsx
+++ b/LocalizationTest.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jerrylee/Projects/Github/UniSharper/UniSharper.Localization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jerry/Projects/GitHub/UniSharper.Localization/develop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E182C941-6417-8E46-A16C-4646D447D43A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15ED3D59-B294-184E-8613-B7D00E2A06AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="1400" windowWidth="30940" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2960" yWindow="1420" windowWidth="33000" windowHeight="18040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Module1" sheetId="1" r:id="rId1"/>
+    <sheet name="Module2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>zh_CN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,17 +90,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>zh-TW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>en</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>nl-be</t>
-  </si>
-  <si>
     <t>LoveYou</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -122,24 +126,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Dutch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hallo!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bedankt.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tot ziens.</t>
-  </si>
-  <si>
-    <t>Ik hou van je.</t>
-  </si>
-  <si>
     <t>locale</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -157,6 +143,89 @@
   </si>
   <si>
     <t>我爱你</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zh_CN.Font</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>en.Font</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>en.Style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zh_CN.Style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zh_TW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zh_TW.Font</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zh_TW.Style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>es_ES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>¡Adiós!</t>
+  </si>
+  <si>
+    <t>¡Te quiero!</t>
+  </si>
+  <si>
+    <t>¡Hola!</t>
+  </si>
+  <si>
+    <t>¡Gracias!</t>
+  </si>
+  <si>
+    <t>es_ES.Font</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>es_ES.Style</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LiberationSans SDF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tanks SDF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tanks Atlas Material|Dark to Light Green - Vertical|42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LiberationSans SDF Material|Blue to Purple - Vertical|40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tanks Atlas Material|Light to Dark Green - Vertical|48</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LiberationSans SDF Material|Yellow to Orange - Vertical|36</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -187,7 +256,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,7 +265,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,17 +300,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -504,11 +604,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21"/>
@@ -517,48 +619,79 @@
     <col min="2" max="2" width="23.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="29.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.83203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="27.1640625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="21.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="29.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="70" style="1" customWidth="1"/>
+    <col min="12" max="12" width="64.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="66.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="79" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="5" customFormat="1">
+      <c r="B2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1">
-      <c r="B2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -573,12 +706,36 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -593,47 +750,31 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.25" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="22">
-      <c r="A6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -641,4 +782,107 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29894EA9-3339-AB42-B525-0C262901EA50}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="25.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="8" customFormat="1" ht="21">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="21">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="22">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>